<commit_message>
various extra files generated while building 3 x v3.2 clocks
</commit_message>
<xml_diff>
--- a/docs/clock3.2_bom.xlsx
+++ b/docs/clock3.2_bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\Arduino\theClock3\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD15794-83AD-4324-A3B2-7A66BED7FBE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07B6C0C-66CF-4099-ACFF-0044177EBBB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2025" yWindow="0" windowWidth="15570" windowHeight="15180" xr2:uid="{090DE66E-4BF6-4DD1-8D36-84EE8FCE0E16}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="98">
   <si>
     <t>Major Wood</t>
   </si>
@@ -321,6 +321,15 @@
   </si>
   <si>
     <t>Bearing, 394</t>
+  </si>
+  <si>
+    <t>6mm diametric magnet</t>
+  </si>
+  <si>
+    <t>included with as5600 sensors</t>
+  </si>
+  <si>
+    <t>pcb, sensor</t>
   </si>
 </sst>
 </file>
@@ -681,8 +690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63EF5283-DEF6-404A-BE77-241F677709E4}">
   <dimension ref="A4:F102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1126,10 +1135,10 @@
         <v>45</v>
       </c>
       <c r="D61">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F61" t="s">
-        <v>46</v>
+        <v>97</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -1435,20 +1444,31 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>86</v>
+        <v>95</v>
+      </c>
+      <c r="D97">
+        <v>3</v>
       </c>
       <c r="F97" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
+        <v>86</v>
+      </c>
+      <c r="F98" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
         <v>88</v>
       </c>
-      <c r="D98">
-        <v>1</v>
-      </c>
-      <c r="E98" s="2">
+      <c r="D99">
+        <v>1</v>
+      </c>
+      <c r="E99" s="2">
         <v>7</v>
       </c>
     </row>
@@ -1458,7 +1478,7 @@
       </c>
       <c r="D102">
         <f>SUM(D6:D100)</f>
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="E102" s="2">
         <f>SUM(E6:E100)</f>

</xml_diff>